<commit_message>
RTL Updates:    - fixed unintended latch bug in PWM module on pwm_out_comb Verification Updates:    - fixed many problems of synchronization between model and RTL
</commit_message>
<xml_diff>
--- a/RTL/DCO/DCO_out_freq_calculator.xlsx
+++ b/RTL/DCO/DCO_out_freq_calculator.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rosuv\Desktop\Disertatie\RISC-V_Microcontroller\RTL\DCO\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE7FA3A2-A507-415E-ABBD-669449D8C3CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{164F1E82-72F9-4EDA-8193-067163EE5CAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-45" yWindow="1620" windowWidth="14730" windowHeight="11385" xr2:uid="{C69D459B-0367-4BC5-B96E-7DE362EF384B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{C69D459B-0367-4BC5-B96E-7DE362EF384B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -93,7 +93,7 @@
     <t>real_out_freq</t>
   </si>
   <si>
-    <t>{USESCLK,CLKSRC}</t>
+    <t>CLKSRC</t>
   </si>
 </sst>
 </file>
@@ -779,7 +779,7 @@
   <dimension ref="A1:H14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+      <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
RTL Updates:    -Fixed bug in PWM/TMR modules in which SW settable only bits were cleared by software    -Updated Excel for DCO/PWM/Timer calculators
Verification Updates:
   -Implemented new system level test scenarios test_prog_03 and test_prog_02
</commit_message>
<xml_diff>
--- a/RTL/DCO/DCO_out_freq_calculator.xlsx
+++ b/RTL/DCO/DCO_out_freq_calculator.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rosuv\Desktop\Disertatie\RISC-V_Microcontroller\RTL\DCO\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{164F1E82-72F9-4EDA-8193-067163EE5CAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7422BDBC-F926-41A9-BB5B-B182031CAC2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{C69D459B-0367-4BC5-B96E-7DE362EF384B}"/>
+    <workbookView xWindow="12750" yWindow="1770" windowWidth="15765" windowHeight="14490" xr2:uid="{C69D459B-0367-4BC5-B96E-7DE362EF384B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="21">
   <si>
     <t>Sys</t>
   </si>
@@ -87,13 +87,19 @@
     <t>out_freq</t>
   </si>
   <si>
-    <t>in_freq</t>
-  </si>
-  <si>
-    <t>real_out_freq</t>
-  </si>
-  <si>
     <t>CLKSRC</t>
+  </si>
+  <si>
+    <t>real_out_freq [Hz]</t>
+  </si>
+  <si>
+    <t>out_freq [Hz]</t>
+  </si>
+  <si>
+    <t>in_freq [Hz]</t>
+  </si>
+  <si>
+    <t>Relative Error [%]</t>
   </si>
 </sst>
 </file>
@@ -149,7 +155,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="19">
+  <borders count="20">
     <border>
       <left/>
       <right/>
@@ -363,17 +369,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
@@ -397,13 +392,37 @@
       <bottom style="medium">
         <color indexed="64"/>
       </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
@@ -413,7 +432,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -436,12 +454,16 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -776,10 +798,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3938274F-0460-433F-8354-BA817FD83B81}">
-  <dimension ref="A1:H14"/>
+  <dimension ref="A1:H15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+      <selection activeCell="J18" sqref="J18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -803,51 +825,51 @@
       <c r="B2" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="11" t="s">
+      <c r="C2" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="12" t="s">
+      <c r="D2" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="12" t="s">
+      <c r="E2" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="F2" s="12" t="s">
+      <c r="F2" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="G2" s="13" t="s">
+      <c r="G2" s="12" t="s">
         <v>9</v>
       </c>
       <c r="H2" s="1"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
-      <c r="B3" s="14" t="s">
+      <c r="B3" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="C3" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="9" t="s">
+      <c r="D3" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="E3" s="9" t="s">
+      <c r="E3" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="F3" s="9" t="s">
+      <c r="F3" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="G3" s="10" t="s">
+      <c r="G3" s="9" t="s">
         <v>4</v>
       </c>
       <c r="H3" s="1"/>
     </row>
     <row r="4" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
-      <c r="B4" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="C4" s="4">
+      <c r="B4" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" s="21">
         <v>1000000</v>
       </c>
       <c r="D4" s="2">
@@ -870,145 +892,172 @@
     </row>
     <row r="5" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1"/>
-      <c r="B5" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="C5" s="7">
-        <v>25000</v>
-      </c>
-      <c r="D5" s="17" t="s">
+      <c r="B5" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" s="24">
+        <v>1000</v>
+      </c>
+      <c r="D5" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="E5" s="18">
+      <c r="E5" s="17">
         <v>20</v>
       </c>
-      <c r="F5" s="20" t="s">
+      <c r="F5" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="G5" s="19"/>
+      <c r="G5" s="18"/>
       <c r="H5" s="1"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
-      <c r="B6" s="15" t="s">
+      <c r="B6" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="6">
+      <c r="C6" s="23">
         <f>IF(AND(((C4/(2*$C$5))-1)&lt;(2^$E$5),((C4/(2*$C$5))-1)&gt;=0),ROUND(((C4/(2*$C$5))-1),0),"Impossible")</f>
-        <v>19</v>
+        <v>499</v>
       </c>
       <c r="D6" s="6">
         <f t="shared" ref="D6:G6" si="1">IF(AND(((D4/(2*$C$5))-1)&lt;(2^$E$5),((D4/(2*$C$5))-1)&gt;=0),ROUND(((D4/(2*$C$5))-1),0),"Impossible")</f>
-        <v>9</v>
+        <v>249</v>
       </c>
       <c r="E6" s="6">
         <f t="shared" si="1"/>
-        <v>4</v>
+        <v>124</v>
       </c>
       <c r="F6" s="6">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>62</v>
       </c>
       <c r="G6" s="6">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="H6" s="1"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
-      <c r="B7" s="15" t="s">
+      <c r="B7" s="14" t="s">
         <v>17</v>
       </c>
       <c r="C7" s="4">
         <f>C4/((C6+1)*2)</f>
-        <v>25000</v>
+        <v>1000</v>
       </c>
       <c r="D7" s="4">
         <f t="shared" ref="D7:G7" si="2">D4/((D6+1)*2)</f>
-        <v>25000</v>
+        <v>1000</v>
       </c>
       <c r="E7" s="4">
         <f t="shared" si="2"/>
-        <v>25000</v>
+        <v>1000</v>
       </c>
       <c r="F7" s="4">
         <f t="shared" si="2"/>
-        <v>20833.333333333332</v>
+        <v>992.06349206349205</v>
       </c>
       <c r="G7" s="4">
         <f t="shared" si="2"/>
-        <v>31250</v>
+        <v>1008.0645161290323</v>
       </c>
       <c r="H7" s="1"/>
     </row>
-    <row r="8" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
-      <c r="B8" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="C8" s="21" t="str">
+      <c r="B8" s="20" t="s">
+        <v>20</v>
+      </c>
+      <c r="C8" s="21">
+        <f>((C7-$C$5)/$C$5)*100</f>
+        <v>0</v>
+      </c>
+      <c r="D8" s="21">
+        <f t="shared" ref="D8:G8" si="3">((D7-$C$5)/$C$5)*100</f>
+        <v>0</v>
+      </c>
+      <c r="E8" s="21">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="F8" s="21">
+        <f t="shared" si="3"/>
+        <v>-0.79365079365079516</v>
+      </c>
+      <c r="G8" s="21">
+        <f t="shared" si="3"/>
+        <v>0.80645161290323131</v>
+      </c>
+      <c r="H8" s="1"/>
+    </row>
+    <row r="9" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="1"/>
+      <c r="B9" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" s="22" t="str">
         <f>DEC2BIN(0,3)</f>
         <v>000</v>
       </c>
-      <c r="D8" s="21" t="str">
+      <c r="D9" s="22" t="str">
         <f>DEC2BIN(1,3)</f>
         <v>001</v>
       </c>
-      <c r="E8" s="21" t="str">
+      <c r="E9" s="22" t="str">
         <f>DEC2BIN(2,3)</f>
         <v>010</v>
       </c>
-      <c r="F8" s="21" t="str">
+      <c r="F9" s="22" t="str">
         <f>DEC2BIN(3,3)</f>
         <v>011</v>
       </c>
-      <c r="G8" s="21" t="str">
+      <c r="G9" s="22" t="str">
         <f>DEC2BIN(4,3)</f>
         <v>100</v>
       </c>
-      <c r="H8" s="1"/>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="1"/>
-      <c r="B9" s="1"/>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
-      <c r="F9" s="1"/>
-      <c r="G9" s="1"/>
       <c r="H9" s="1"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B13" t="s">
-        <v>11</v>
-      </c>
-      <c r="C13">
-        <v>2</v>
-      </c>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="1"/>
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
+        <v>11</v>
+      </c>
+      <c r="C14">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
         <v>15</v>
       </c>
-      <c r="C14">
-        <f>C4/(($C$13+1)*2)</f>
+      <c r="C15">
+        <f>C4/(($C$14+1)*2)</f>
         <v>166666.66666666666</v>
       </c>
-      <c r="D14">
-        <f t="shared" ref="D14:G14" si="3">D4/(($C$13+1)*2)</f>
+      <c r="D15">
+        <f t="shared" ref="D15:G15" si="4">D4/(($C$14+1)*2)</f>
         <v>83333.333333333328</v>
       </c>
-      <c r="E14">
-        <f t="shared" si="3"/>
+      <c r="E15">
+        <f t="shared" si="4"/>
         <v>41666.666666666664</v>
       </c>
-      <c r="F14">
-        <f t="shared" si="3"/>
+      <c r="F15">
+        <f t="shared" si="4"/>
         <v>20833.333333333332</v>
       </c>
-      <c r="G14">
-        <f t="shared" si="3"/>
+      <c r="G15">
+        <f t="shared" si="4"/>
         <v>10416.666666666666</v>
       </c>
     </row>

</xml_diff>